<commit_message>
Fixed SA and Overall score data, also added configuration as the x label to all plots.
</commit_message>
<xml_diff>
--- a/Scoring_SHADOW/SART with averages and rounding.xlsx
+++ b/Scoring_SHADOW/SART with averages and rounding.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/coolhomie1987/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049E01C7-AAD0-6744-B70E-D58F601164BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07FB98D-C9B3-A747-9796-031DD80C6C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1860" windowWidth="27640" windowHeight="16940" xr2:uid="{8F7E6633-DC76-BE4A-AB1E-19930F50F8C1}"/>
+    <workbookView xWindow="4500" yWindow="1160" windowWidth="27640" windowHeight="16940" xr2:uid="{8F7E6633-DC76-BE4A-AB1E-19930F50F8C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -83,43 +83,19 @@
     <t>SART</t>
   </si>
   <si>
-    <t>Assassin</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
     <t>AA</t>
   </si>
   <si>
-    <t>Chuck</t>
-  </si>
-  <si>
-    <t>Indy</t>
-  </si>
-  <si>
-    <t>MACH</t>
-  </si>
-  <si>
     <t>AVG</t>
-  </si>
-  <si>
-    <t>Tars</t>
-  </si>
-  <si>
-    <t>Pig</t>
-  </si>
-  <si>
-    <t>Savage</t>
   </si>
   <si>
     <t>AH</t>
   </si>
   <si>
     <t>HA</t>
-  </si>
-  <si>
-    <t>Mach</t>
   </si>
   <si>
     <t>HH</t>
@@ -144,6 +120,27 @@
   </si>
   <si>
     <t>SART (Rounded After)</t>
+  </si>
+  <si>
+    <t>Grimmer</t>
+  </si>
+  <si>
+    <t>McIntyre</t>
+  </si>
+  <si>
+    <t>Fleischmann</t>
+  </si>
+  <si>
+    <t>Schnell</t>
+  </si>
+  <si>
+    <t>Chan</t>
+  </si>
+  <si>
+    <t>Jacob</t>
+  </si>
+  <si>
+    <t>Smith</t>
   </si>
 </sst>
 </file>
@@ -229,24 +226,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="25">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -358,6 +337,24 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -905,7 +902,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D0510FEC-765E-FE4A-9CA1-B5FF96AA12CF}" name="Table2" displayName="Table2" ref="A1:V29" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="A1:V29" xr:uid="{D0510FEC-765E-FE4A-9CA1-B5FF96AA12CF}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:V29">
-    <sortCondition ref="D1:D29"/>
+    <sortCondition descending="1" ref="D1:D29"/>
   </sortState>
   <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{EEA55536-968C-5F41-8999-71B41D6029B0}" name="Name" dataDxfId="21"/>
@@ -922,14 +919,28 @@
     <tableColumn id="12" xr3:uid="{71BFE439-6408-DD47-A4C6-DBD79B673DDB}" name="INFORMATION QUANTITY" dataDxfId="10"/>
     <tableColumn id="13" xr3:uid="{B5DC5E7E-ECB6-034C-B7F9-5E38F7E3DDE4}" name="INFORMATION QUALITY" dataDxfId="9"/>
     <tableColumn id="14" xr3:uid="{61548AFD-A529-CC46-AA12-FEB70D2F880F}" name="FAMILIARITY WITH SITUATION" dataDxfId="8"/>
-    <tableColumn id="21" xr3:uid="{A48DD5DC-A236-3948-AD72-D9D03C267E85}" name="Demand (Unrounded)" dataDxfId="1"/>
-    <tableColumn id="20" xr3:uid="{17D793A5-2DD9-8849-B1D0-B35B970CB7F7}" name="Supply (Unrounded)" dataDxfId="2"/>
-    <tableColumn id="19" xr3:uid="{4252D25F-CA61-384A-AB1B-435882C846ED}" name="Understanding (Unrounded)" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{FE452DB1-4337-9441-AC9C-32098254A9B8}" name="SART (Rounded After)" dataDxfId="0"/>
-    <tableColumn id="15" xr3:uid="{8578A6B0-D16F-C940-98C7-72D4F83319E5}" name="Demand (Rounded)" dataDxfId="7"/>
-    <tableColumn id="16" xr3:uid="{CFD3A10E-8725-3845-A923-888A7E4D68C9}" name="Supply (Rounded)" dataDxfId="6"/>
-    <tableColumn id="17" xr3:uid="{7D542867-5511-6944-888F-15C8E61D5116}" name="Understanding (Rounded)" dataDxfId="5"/>
-    <tableColumn id="18" xr3:uid="{4F835F49-0A00-2C45-A861-80CA437CD370}" name="SART" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{A48DD5DC-A236-3948-AD72-D9D03C267E85}" name="Demand (Unrounded)" dataDxfId="7">
+      <calculatedColumnFormula>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="20" xr3:uid="{17D793A5-2DD9-8849-B1D0-B35B970CB7F7}" name="Supply (Unrounded)" dataDxfId="6">
+      <calculatedColumnFormula>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="19" xr3:uid="{4252D25F-CA61-384A-AB1B-435882C846ED}" name="Understanding (Unrounded)" dataDxfId="5">
+      <calculatedColumnFormula>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="22" xr3:uid="{FE452DB1-4337-9441-AC9C-32098254A9B8}" name="SART (Rounded After)" dataDxfId="4">
+      <calculatedColumnFormula>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{8578A6B0-D16F-C940-98C7-72D4F83319E5}" name="Demand (Rounded)" dataDxfId="3">
+      <calculatedColumnFormula>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{CFD3A10E-8725-3845-A923-888A7E4D68C9}" name="Supply (Rounded)" dataDxfId="2">
+      <calculatedColumnFormula>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="17" xr3:uid="{7D542867-5511-6944-888F-15C8E61D5116}" name="Understanding (Rounded)" dataDxfId="1"/>
+    <tableColumn id="18" xr3:uid="{4F835F49-0A00-2C45-A861-80CA437CD370}" name="SART" dataDxfId="0">
+      <calculatedColumnFormula>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1254,8 +1265,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4031D9-897F-194D-A272-A2F02105F795}">
   <dimension ref="A1:V29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="N1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1322,25 +1334,25 @@
         <v>13</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="6" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="T1" s="4" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>14</v>
@@ -1348,164 +1360,180 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="1">
-        <v>45916</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2">
         <v>2</v>
       </c>
       <c r="H2" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I2" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J2" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K2" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L2" s="2">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="M2" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N2" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O2" s="5">
-        <v>2</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="P2" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4.5</v>
       </c>
       <c r="Q2" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>4.5</v>
       </c>
       <c r="R2" s="5">
-        <v>4</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="S2" s="2">
-        <v>2</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="T2" s="2">
-        <v>3</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="U2" s="2">
-        <v>3</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="V2" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
-        <v>45912</v>
+        <v>45915</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G3" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H3" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I3" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J3" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="K3" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L3" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M3" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N3" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O3" s="5">
-        <v>2</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="P3" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4.5</v>
       </c>
       <c r="Q3" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
         <v>3</v>
       </c>
       <c r="R3" s="5">
-        <v>4</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>1</v>
       </c>
       <c r="S3" s="2">
-        <v>2</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="T3" s="2">
-        <v>3</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="U3" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
         <v>3</v>
       </c>
       <c r="V3" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45911</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="E4" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F4" s="2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="G4" s="2">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="H4" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I4" s="2">
         <v>5</v>
@@ -1514,193 +1542,217 @@
         <v>3</v>
       </c>
       <c r="K4" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="L4" s="2">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="M4" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N4" s="2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="O4" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3.5</v>
       </c>
       <c r="P4" s="5">
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
         <v>4.5</v>
       </c>
       <c r="Q4" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5.5</v>
       </c>
       <c r="R4" s="5">
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>6</v>
       </c>
       <c r="S4" s="2">
-        <v>3</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="T4" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U4" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V4" s="2">
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="1">
+        <v>45912</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="E5" s="2">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="F5" s="2">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="G5" s="2">
-        <v>3.25</v>
+        <v>2</v>
       </c>
       <c r="H5" s="2">
-        <v>4.75</v>
+        <v>4</v>
       </c>
       <c r="I5" s="2">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="J5" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="K5" s="2">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="L5" s="2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="M5" s="2">
-        <v>5.75</v>
+        <v>6</v>
       </c>
       <c r="N5" s="2">
-        <v>5.25</v>
+        <v>5</v>
       </c>
       <c r="O5" s="5">
-        <v>3.25</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>2</v>
       </c>
       <c r="P5" s="5">
-        <v>4.625</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4</v>
       </c>
       <c r="Q5" s="5">
-        <v>4.625</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5</v>
       </c>
       <c r="R5" s="5">
-        <v>6</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>7</v>
       </c>
       <c r="S5" s="2">
-        <v>4</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>2</v>
       </c>
       <c r="T5" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U5" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V5" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1">
-        <v>45916</v>
+        <v>45912</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2">
         <v>3</v>
       </c>
       <c r="F6" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G6" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H6" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J6" s="2">
         <v>4</v>
       </c>
       <c r="K6" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L6" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M6" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N6" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O6" s="5">
-        <v>3.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="P6" s="5">
-        <v>5.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4.5</v>
       </c>
       <c r="Q6" s="5">
-        <v>5.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="R6" s="5">
-        <v>7</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="S6" s="2">
-        <v>3</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="T6" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U6" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="V6" s="2">
-        <v>5</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B7" s="1">
-        <v>45912</v>
+        <v>45910</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" s="2">
         <v>4</v>
@@ -1709,152 +1761,168 @@
         <v>3</v>
       </c>
       <c r="H7" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I7" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J7" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K7" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L7" s="2">
         <v>6</v>
       </c>
       <c r="M7" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N7" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="O7" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="P7" s="5">
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
         <v>4</v>
       </c>
       <c r="Q7" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="R7" s="5">
-        <v>5</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="S7" s="2">
-        <v>3</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="T7" s="2">
-        <v>3</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="U7" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
         <v>3</v>
       </c>
       <c r="V7" s="2">
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
+      </c>
+      <c r="B8" s="1">
+        <v>45916</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E8" s="2">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="F8" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="2">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="H8" s="2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="I8" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J8" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K8" s="2">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="L8" s="2">
         <v>5</v>
       </c>
       <c r="M8" s="2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="N8" s="2">
-        <v>5.5</v>
+        <v>4</v>
       </c>
       <c r="O8" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>2</v>
       </c>
       <c r="P8" s="5">
-        <v>3.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4.5</v>
       </c>
       <c r="Q8" s="5">
-        <v>3.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5</v>
       </c>
       <c r="R8" s="5">
-        <v>4</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>7</v>
       </c>
       <c r="S8" s="2">
-        <v>4</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>2</v>
       </c>
       <c r="T8" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="U8" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
         <v>5</v>
       </c>
       <c r="V8" s="2">
-        <v>6</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45911</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1">
-        <v>45916</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D9" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E9" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F9" s="2">
         <v>3</v>
       </c>
       <c r="G9" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H9" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I9" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J9" s="2">
         <v>5</v>
       </c>
       <c r="K9" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L9" s="2">
         <v>4</v>
@@ -1863,258 +1931,290 @@
         <v>4</v>
       </c>
       <c r="N9" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O9" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
         <v>3</v>
       </c>
       <c r="P9" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>5.5</v>
       </c>
       <c r="Q9" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="R9" s="5">
-        <v>7</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="S9" s="2">
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>3</v>
       </c>
       <c r="T9" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>5</v>
       </c>
       <c r="U9" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="V9" s="2">
-        <v>7</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1">
-        <v>45912</v>
+        <v>45915</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F10" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G10" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H10" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I10" s="2">
         <v>4</v>
       </c>
       <c r="J10" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K10" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L10" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M10" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N10" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="O10" s="5">
-        <v>6</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="P10" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4</v>
       </c>
       <c r="Q10" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="R10" s="5">
-        <v>3</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="S10" s="2">
-        <v>6</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="T10" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U10" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="V10" s="2">
-        <v>2</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
-        <v>19</v>
+      <c r="A11" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B11" s="1">
         <v>45911</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E11" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F11" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H11" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I11" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J11" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K11" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L11" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M11" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N11" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O11" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="P11" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>5</v>
       </c>
       <c r="Q11" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="R11" s="5">
-        <v>5</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>7</v>
       </c>
       <c r="S11" s="2">
-        <v>3</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="T11" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="U11" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="V11" s="2">
-        <v>5</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="1">
-        <v>45910</v>
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E12" s="2">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="F12" s="2">
         <v>4</v>
       </c>
       <c r="G12" s="2">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="H12" s="2">
         <v>6</v>
       </c>
       <c r="I12" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J12" s="2">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="K12" s="2">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="L12" s="2">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="M12" s="2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="N12" s="2">
-        <v>3</v>
+        <v>4.5</v>
       </c>
       <c r="O12" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>5.5</v>
       </c>
       <c r="P12" s="5">
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
         <v>5</v>
       </c>
       <c r="Q12" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>3.5</v>
       </c>
       <c r="R12" s="5">
-        <v>6</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="S12" s="2">
-        <v>4</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="T12" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>5</v>
       </c>
       <c r="U12" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="V12" s="2">
-        <v>6</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1">
-        <v>45916</v>
+        <v>45912</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E13" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G13" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H13" s="2">
         <v>5</v>
@@ -2123,199 +2223,223 @@
         <v>5</v>
       </c>
       <c r="J13" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K13" s="2">
         <v>3</v>
       </c>
       <c r="L13" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M13" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N13" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="O13" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>5</v>
       </c>
       <c r="P13" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4.5</v>
       </c>
       <c r="Q13" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="R13" s="5">
-        <v>7</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="S13" s="2">
-        <v>3</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="T13" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="U13" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="V13" s="2">
-        <v>7</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="1">
-        <v>45912</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E14" s="2">
-        <v>3</v>
-      </c>
-      <c r="F14" s="2">
-        <v>4</v>
-      </c>
-      <c r="G14" s="2">
-        <v>4</v>
-      </c>
-      <c r="H14" s="2">
-        <v>4</v>
-      </c>
-      <c r="I14" s="2">
-        <v>3</v>
-      </c>
-      <c r="J14" s="2">
-        <v>3</v>
-      </c>
-      <c r="K14" s="2">
-        <v>5</v>
-      </c>
-      <c r="L14" s="2">
-        <v>5</v>
-      </c>
-      <c r="M14" s="2">
-        <v>6</v>
-      </c>
-      <c r="N14" s="2">
-        <v>7</v>
+        <v>31</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="F14" s="3">
+        <v>4.5</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4</v>
+      </c>
+      <c r="I14" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="K14" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="L14" s="3">
+        <v>6</v>
+      </c>
+      <c r="M14" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="N14" s="3">
+        <v>3.5</v>
       </c>
       <c r="O14" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>4.5</v>
       </c>
       <c r="P14" s="5">
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>3.75</v>
+      </c>
+      <c r="Q14" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
         <v>3.5</v>
       </c>
-      <c r="Q14" s="5">
-        <v>3.5</v>
-      </c>
       <c r="R14" s="5">
-        <v>3</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>2</v>
       </c>
       <c r="S14" s="2">
-        <v>4</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="T14" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>3</v>
       </c>
       <c r="U14" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
         <v>3</v>
       </c>
       <c r="V14" s="2">
-        <v>2</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B15" s="1">
-        <v>45912</v>
+        <v>45916</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F15" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G15" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H15" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I15" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J15" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K15" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L15" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M15" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N15" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O15" s="5">
-        <v>3</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>2</v>
       </c>
       <c r="P15" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4</v>
       </c>
       <c r="Q15" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5</v>
       </c>
       <c r="R15" s="5">
-        <v>6</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>7</v>
       </c>
       <c r="S15" s="2">
-        <v>3</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>2</v>
       </c>
       <c r="T15" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U15" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V15" s="2">
-        <v>5</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="1">
+        <v>45911</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
-        <v>45916</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F16" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G16" s="2">
         <v>2</v>
@@ -2327,125 +2451,141 @@
         <v>4</v>
       </c>
       <c r="J16" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K16" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L16" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M16" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N16" s="2">
         <v>5</v>
       </c>
       <c r="O16" s="5">
-        <v>5.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="P16" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4</v>
       </c>
       <c r="Q16" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="R16" s="5">
-        <v>4</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="S16" s="2">
-        <v>2</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="T16" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U16" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="V16" s="2">
-        <v>6</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1">
+        <v>45916</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="E17" s="2">
-        <v>6.5</v>
+        <v>3</v>
       </c>
       <c r="F17" s="2">
         <v>4</v>
       </c>
       <c r="G17" s="2">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="H17" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I17" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J17" s="2">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="K17" s="2">
-        <v>5.5</v>
+        <v>3</v>
       </c>
       <c r="L17" s="2">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="M17" s="2">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="N17" s="2">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="O17" s="5">
-        <v>2</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="P17" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>5</v>
       </c>
       <c r="Q17" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
         <v>4</v>
       </c>
       <c r="R17" s="5">
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>6</v>
       </c>
       <c r="S17" s="2">
-        <v>6</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="T17" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>5</v>
       </c>
       <c r="U17" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="V17" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
-        <v>19</v>
+      <c r="A18" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B18" s="1">
-        <v>45911</v>
+        <v>45912</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E18" s="2">
         <v>3</v>
@@ -2454,134 +2594,150 @@
         <v>3</v>
       </c>
       <c r="G18" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H18" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I18" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J18" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="K18" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L18" s="2">
         <v>4</v>
       </c>
       <c r="M18" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N18" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O18" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
         <v>3</v>
       </c>
       <c r="P18" s="5">
-        <v>5.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4.5</v>
       </c>
       <c r="Q18" s="5">
-        <v>5.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="R18" s="5">
-        <v>8</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>7</v>
       </c>
       <c r="S18" s="2">
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>3</v>
       </c>
       <c r="T18" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="U18" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="V18" s="2">
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="A19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" s="1">
+        <v>45912</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="2">
+        <v>6</v>
+      </c>
+      <c r="F19" s="2">
+        <v>2</v>
+      </c>
+      <c r="G19" s="2">
+        <v>6</v>
+      </c>
+      <c r="H19" s="2">
+        <v>5</v>
+      </c>
+      <c r="I19" s="2">
+        <v>4</v>
+      </c>
+      <c r="J19" s="2">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2">
+        <v>6</v>
+      </c>
+      <c r="L19" s="2">
+        <v>5</v>
+      </c>
+      <c r="M19" s="2">
+        <v>6</v>
+      </c>
+      <c r="N19" s="2">
+        <v>2</v>
+      </c>
+      <c r="O19" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>6</v>
+      </c>
+      <c r="P19" s="5">
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
         <v>4.5</v>
       </c>
-      <c r="F19" s="3">
-        <v>4.5</v>
-      </c>
-      <c r="G19" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="H19" s="3">
-        <v>4</v>
-      </c>
-      <c r="I19" s="3">
-        <v>5.5</v>
-      </c>
-      <c r="J19" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="K19" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="L19" s="3">
-        <v>6</v>
-      </c>
-      <c r="M19" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="N19" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="O19" s="5">
-        <v>4.5</v>
-      </c>
-      <c r="P19" s="5">
-        <v>3.75</v>
-      </c>
       <c r="Q19" s="5">
-        <v>3.75</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5</v>
       </c>
       <c r="R19" s="5">
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>3</v>
       </c>
       <c r="S19" s="2">
-        <v>5</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="T19" s="2">
-        <v>3</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="U19" s="2">
-        <v>3</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V19" s="2">
-        <v>1</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1">
-        <v>45915</v>
+        <v>45912</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E20" s="2">
         <v>3</v>
@@ -2596,658 +2752,738 @@
         <v>4</v>
       </c>
       <c r="I20" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J20" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K20" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L20" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M20" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="N20" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O20" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
         <v>4</v>
       </c>
       <c r="P20" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>3.5</v>
       </c>
       <c r="Q20" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="R20" s="5">
-        <v>4</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="S20" s="2">
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="T20" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="U20" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="V20" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1">
-        <v>45912</v>
+        <v>45910</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F21" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H21" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I21" s="2">
         <v>5</v>
       </c>
       <c r="J21" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K21" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L21" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M21" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="N21" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="O21" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="P21" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>5</v>
       </c>
       <c r="Q21" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="R21" s="5">
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="S21" s="2">
-        <v>5</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="T21" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="U21" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="V21" s="2">
-        <v>3</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>4</v>
       </c>
     </row>
     <row r="22" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B22" s="1">
-        <v>45911</v>
+        <v>45916</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E22" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F22" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G22" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H22" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I22" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J22" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K22" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L22" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M22" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N22" s="2">
         <v>6</v>
       </c>
       <c r="O22" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="P22" s="5">
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
         <v>5</v>
       </c>
       <c r="Q22" s="5">
-        <v>5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="R22" s="5">
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>6</v>
       </c>
       <c r="S22" s="2">
-        <v>4</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="T22" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>5</v>
       </c>
       <c r="U22" s="2">
-        <v>5</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="V22" s="2">
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="1">
+        <v>45911</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="1">
-        <v>45916</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G23" s="2">
         <v>2</v>
       </c>
       <c r="H23" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I23" s="2">
         <v>5</v>
       </c>
       <c r="J23" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K23" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L23" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M23" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N23" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="O23" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
         <v>3</v>
       </c>
       <c r="P23" s="5">
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
         <v>4.5</v>
       </c>
       <c r="Q23" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>4</v>
       </c>
       <c r="R23" s="5">
-        <v>6</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="S23" s="2">
-        <v>2</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="T23" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U23" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="V23" s="2">
-        <v>6</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1">
-        <v>45912</v>
+        <v>45916</v>
       </c>
       <c r="C24" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E24" s="2">
         <v>3</v>
       </c>
       <c r="F24" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H24" s="2">
         <v>4</v>
       </c>
       <c r="I24" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J24" s="2">
         <v>4</v>
       </c>
       <c r="K24" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L24" s="2">
         <v>5</v>
       </c>
       <c r="M24" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="N24" s="2">
         <v>5</v>
       </c>
       <c r="O24" s="5">
-        <v>3.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="P24" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4</v>
       </c>
       <c r="Q24" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5</v>
       </c>
       <c r="R24" s="5">
-        <v>5</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="S24" s="2">
-        <v>2</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="T24" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U24" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V24" s="2">
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
         <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>19</v>
+      <c r="A25" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E25" s="2">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="F25" s="2">
         <v>3</v>
       </c>
       <c r="G25" s="2">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="H25" s="2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="I25" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J25" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K25" s="2">
-        <v>3</v>
+        <v>5.5</v>
       </c>
       <c r="L25" s="2">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="M25" s="2">
-        <v>4</v>
+        <v>5.5</v>
       </c>
       <c r="N25" s="2">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="O25" s="5">
-        <v>2</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3.5</v>
       </c>
       <c r="P25" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>5.5</v>
       </c>
       <c r="Q25" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5.5</v>
       </c>
       <c r="R25" s="5">
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>7</v>
       </c>
       <c r="S25" s="2">
-        <v>3</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>4</v>
       </c>
       <c r="T25" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="U25" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V25" s="2">
-        <v>5</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1">
-        <v>45910</v>
+        <v>45912</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E26" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F26" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G26" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H26" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I26" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J26" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K26" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L26" s="2">
         <v>6</v>
       </c>
       <c r="M26" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N26" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="O26" s="5">
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
         <v>2</v>
       </c>
       <c r="P26" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>3</v>
       </c>
       <c r="Q26" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="R26" s="5">
-        <v>6</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>7</v>
       </c>
       <c r="S26" s="2">
-        <v>4</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>2</v>
       </c>
       <c r="T26" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="U26" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="V26" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B27" s="1">
-        <v>45915</v>
+        <v>45912</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E27" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F27" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G27" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H27" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I27" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J27" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="K27" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L27" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="M27" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="N27" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="O27" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3</v>
       </c>
       <c r="P27" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>3.5</v>
       </c>
       <c r="Q27" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>6</v>
       </c>
       <c r="R27" s="5">
-        <v>4</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="S27" s="2">
-        <v>6</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="T27" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="U27" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="V27" s="2">
-        <v>2</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="1">
-        <v>45912</v>
+        <v>31</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E28" s="2">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="F28" s="2">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="G28" s="2">
-        <v>5</v>
+        <v>3.25</v>
       </c>
       <c r="H28" s="2">
-        <v>5</v>
+        <v>4.75</v>
       </c>
       <c r="I28" s="2">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="J28" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="K28" s="2">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="L28" s="2">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="M28" s="2">
-        <v>6</v>
+        <v>5.75</v>
       </c>
       <c r="N28" s="2">
-        <v>7</v>
+        <v>5.25</v>
       </c>
       <c r="O28" s="5">
-        <v>6</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>3.25</v>
       </c>
       <c r="P28" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>4.625</v>
       </c>
       <c r="Q28" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5.5</v>
       </c>
       <c r="R28" s="5">
-        <v>3</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="S28" s="2">
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="T28" s="2">
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
         <v>4</v>
       </c>
       <c r="U28" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V28" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>5</v>
       </c>
     </row>
     <row r="29" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="3" t="s">
+      <c r="A29" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="1">
+        <v>45916</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="E29" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F29" s="2">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="G29" s="2">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="H29" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I29" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J29" s="2">
         <v>3</v>
       </c>
       <c r="K29" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L29" s="2">
-        <v>5.5</v>
+        <v>5</v>
       </c>
       <c r="M29" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N29" s="2">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="O29" s="5">
-        <v>4</v>
+        <f>MEDIAN(Table2[[#This Row],[INSTABILITY OF SITUATION]:[VARIABILITY OF SITUATION]])</f>
+        <v>2</v>
       </c>
       <c r="P29" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[AROUSAL]:[SPARE MENTAL CAPACITY]])</f>
+        <v>3</v>
       </c>
       <c r="Q29" s="5">
-        <v>4.5</v>
+        <f>MEDIAN(Table2[[#This Row],[INFORMATION QUANTITY]:[FAMILIARITY WITH SITUATION]])</f>
+        <v>5</v>
       </c>
       <c r="R29" s="5">
-        <v>5</v>
+        <f>ROUNDDOWN((Table2[[#This Row],[Supply (Unrounded)]]+Table2[[#This Row],[Understanding (Unrounded)]])-Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>6</v>
       </c>
       <c r="S29" s="2">
-        <v>4</v>
+        <f>ROUNDUP(Table2[[#This Row],[Demand (Unrounded)]],0)</f>
+        <v>2</v>
       </c>
       <c r="T29" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Supply (Unrounded)]],0)</f>
+        <v>3</v>
       </c>
       <c r="U29" s="2">
-        <v>4</v>
+        <f>ROUNDDOWN(Table2[[#This Row],[Understanding (Unrounded)]],0)</f>
+        <v>5</v>
       </c>
       <c r="V29" s="2">
-        <v>4</v>
+        <f>(Table2[[#This Row],[Understanding (Rounded)]]+Table2[[#This Row],[Supply (Rounded)]])-Table2[[#This Row],[Demand (Rounded)]]</f>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>